<commit_message>
fix(nfl): recent xlsx not uploaded after page sync
</commit_message>
<xml_diff>
--- a/NFL Barbook Trivia.xlsx
+++ b/NFL Barbook Trivia.xlsx
@@ -11,14 +11,37 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="6fCtRWswlWQMto6z7LwvVwHAuTexYowj9Kh61cpS1Yw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="kIEnLtnbnPk04+87l9+vUD5sgIQQHXoKhbbpNeFsRs0="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="G100">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABzqpGels
+Joe Fortman    (2026-02-28 01:34:23)
+should've said "nfl-qb-passing-leaders-by-team" but editing it is limited to 3 per month so not doing it now</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgf3FIot+Pbr2PXhTPMZ5EVEL6Y3g=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="431">
   <si>
     <t>📚  Page Configuration Editor</t>
   </si>
@@ -962,6 +985,9 @@
     <t>List the top 10 latest-picked players (highest pick number) who made a Pro Bowl.</t>
   </si>
   <si>
+    <t>teams</t>
+  </si>
+  <si>
     <t>NFL — Franchise Leaders: All-Time Passing Yards (32 Teams)</t>
   </si>
   <si>
@@ -969,6 +995,9 @@
   </si>
   <si>
     <t>32 items — clues are team names (all 32)</t>
+  </si>
+  <si>
+    <t>https://bit.ly/nfl-qb-leaders-by-team</t>
   </si>
   <si>
     <t>NFL — Franchise Leaders: All-Time Rushing Yards (32 Teams)</t>
@@ -1315,7 +1344,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1388,6 +1417,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="10.0"/>
+      <color rgb="FF38761D"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u/>
       <sz val="9.0"/>
       <color rgb="FF2563EB"/>
@@ -1430,7 +1465,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1471,6 +1506,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE7F3"/>
         <bgColor rgb="FFFCE7F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
@@ -1548,7 +1589,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1605,50 +1646,53 @@
     <xf borderId="4" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="8" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="7" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="7" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="9" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="9" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="9" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="10" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="11" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1887,7 +1931,7 @@
     <col customWidth="1" min="7" max="7" width="50.0"/>
     <col customWidth="1" min="8" max="8" width="36.0"/>
     <col customWidth="1" min="9" max="10" width="14.0"/>
-    <col customWidth="1" min="11" max="11" width="10.0"/>
+    <col customWidth="1" min="11" max="11" width="9.43"/>
     <col customWidth="1" min="12" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -4568,22 +4612,24 @@
       <c r="A100" s="16">
         <v>96.0</v>
       </c>
-      <c r="B100" s="17" t="s">
-        <v>13</v>
+      <c r="B100" s="20" t="s">
+        <v>314</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F100" s="18">
         <v>2.0</v>
       </c>
-      <c r="G100" s="19"/>
+      <c r="G100" s="19" t="s">
+        <v>318</v>
+      </c>
       <c r="H100" s="8"/>
       <c r="I100" s="10"/>
       <c r="J100" s="10"/>
@@ -4593,17 +4639,17 @@
       <c r="A101" s="16">
         <v>97.0</v>
       </c>
-      <c r="B101" s="17" t="s">
-        <v>13</v>
+      <c r="B101" s="20" t="s">
+        <v>314</v>
       </c>
       <c r="C101" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E101" s="18" t="s">
         <v>317</v>
-      </c>
-      <c r="D101" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="E101" s="18" t="s">
-        <v>316</v>
       </c>
       <c r="F101" s="18">
         <v>2.0</v>
@@ -4618,17 +4664,17 @@
       <c r="A102" s="16">
         <v>98.0</v>
       </c>
-      <c r="B102" s="17" t="s">
-        <v>13</v>
+      <c r="B102" s="20" t="s">
+        <v>314</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F102" s="18">
         <v>2.0</v>
@@ -4647,10 +4693,10 @@
         <v>13</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E103" s="18" t="s">
         <v>78</v>
@@ -4659,7 +4705,7 @@
         <v>1.0</v>
       </c>
       <c r="G103" s="19" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H103" s="8"/>
       <c r="I103" s="10"/>
@@ -4674,10 +4720,10 @@
         <v>13</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E104" s="18" t="s">
         <v>78</v>
@@ -4686,7 +4732,7 @@
         <v>1.0</v>
       </c>
       <c r="G104" s="19" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="H104" s="8"/>
       <c r="I104" s="10"/>
@@ -4701,10 +4747,10 @@
         <v>13</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E105" s="18" t="s">
         <v>78</v>
@@ -4713,7 +4759,7 @@
         <v>1.0</v>
       </c>
       <c r="G105" s="19" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="H105" s="8"/>
       <c r="I105" s="10"/>
@@ -4728,7 +4774,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D106" s="18" t="s">
         <v>237</v>
@@ -4755,10 +4801,10 @@
         <v>13</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E107" s="18" t="s">
         <v>78</v>
@@ -4767,7 +4813,7 @@
         <v>1.0</v>
       </c>
       <c r="G107" s="19" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="10"/>
@@ -4782,10 +4828,10 @@
         <v>13</v>
       </c>
       <c r="C108" s="18" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E108" s="18" t="s">
         <v>78</v>
@@ -4794,7 +4840,7 @@
         <v>1.0</v>
       </c>
       <c r="G108" s="19" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="H108" s="8"/>
       <c r="I108" s="10"/>
@@ -4809,10 +4855,10 @@
         <v>13</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E109" s="18" t="s">
         <v>73</v>
@@ -4821,7 +4867,7 @@
         <v>1.0</v>
       </c>
       <c r="G109" s="19" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="H109" s="8"/>
       <c r="I109" s="10"/>
@@ -4836,10 +4882,10 @@
         <v>13</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E110" s="18" t="s">
         <v>73</v>
@@ -4848,7 +4894,7 @@
         <v>1.0</v>
       </c>
       <c r="G110" s="19" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="H110" s="8"/>
       <c r="I110" s="10"/>
@@ -4863,10 +4909,10 @@
         <v>13</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E111" s="18" t="s">
         <v>73</v>
@@ -4875,7 +4921,7 @@
         <v>1.0</v>
       </c>
       <c r="G111" s="19" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="H111" s="8"/>
       <c r="I111" s="10"/>
@@ -4890,10 +4936,10 @@
         <v>13</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>73</v>
@@ -4902,7 +4948,7 @@
         <v>1.0</v>
       </c>
       <c r="G112" s="19" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="H112" s="8"/>
       <c r="I112" s="10"/>
@@ -4917,10 +4963,10 @@
         <v>13</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E113" s="18" t="s">
         <v>73</v>
@@ -4929,7 +4975,7 @@
         <v>1.0</v>
       </c>
       <c r="G113" s="19" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="H113" s="8"/>
       <c r="I113" s="10"/>
@@ -4944,10 +4990,10 @@
         <v>13</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E114" s="18" t="s">
         <v>73</v>
@@ -4956,7 +5002,7 @@
         <v>1.0</v>
       </c>
       <c r="G114" s="19" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="H114" s="8"/>
       <c r="I114" s="10"/>
@@ -4971,10 +5017,10 @@
         <v>13</v>
       </c>
       <c r="C115" s="18" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E115" s="18" t="s">
         <v>73</v>
@@ -4982,8 +5028,8 @@
       <c r="F115" s="18">
         <v>1.0</v>
       </c>
-      <c r="G115" s="20" t="s">
-        <v>357</v>
+      <c r="G115" s="21" t="s">
+        <v>359</v>
       </c>
       <c r="H115" s="8"/>
       <c r="I115" s="10"/>
@@ -4998,10 +5044,10 @@
         <v>13</v>
       </c>
       <c r="C116" s="18" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E116" s="18" t="s">
         <v>73</v>
@@ -5010,7 +5056,7 @@
         <v>1.0</v>
       </c>
       <c r="G116" s="19" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="H116" s="8"/>
       <c r="I116" s="10"/>
@@ -5897,107 +5943,108 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" location="fantasy::27" ref="G18"/>
-    <hyperlink r:id="rId2" ref="G19"/>
-    <hyperlink r:id="rId3" ref="G20"/>
-    <hyperlink r:id="rId4" ref="G21"/>
-    <hyperlink r:id="rId5" ref="G22"/>
-    <hyperlink r:id="rId6" ref="G23"/>
-    <hyperlink r:id="rId7" ref="G24"/>
-    <hyperlink r:id="rId8" ref="G25"/>
-    <hyperlink r:id="rId9" ref="G26"/>
-    <hyperlink r:id="rId10" ref="G27"/>
-    <hyperlink r:id="rId11" ref="G28"/>
-    <hyperlink r:id="rId12" ref="G29"/>
-    <hyperlink r:id="rId13" ref="G30"/>
-    <hyperlink r:id="rId14" ref="G31"/>
-    <hyperlink r:id="rId15" ref="G32"/>
-    <hyperlink r:id="rId16" ref="G33"/>
-    <hyperlink r:id="rId17" ref="G34"/>
-    <hyperlink r:id="rId18" ref="G35"/>
-    <hyperlink r:id="rId19" ref="G36"/>
-    <hyperlink r:id="rId20" ref="G37"/>
-    <hyperlink r:id="rId21" ref="G38"/>
-    <hyperlink r:id="rId22" ref="G39"/>
-    <hyperlink r:id="rId23" ref="G40"/>
-    <hyperlink r:id="rId24" ref="G41"/>
-    <hyperlink r:id="rId25" ref="G42"/>
-    <hyperlink r:id="rId26" ref="G43"/>
-    <hyperlink r:id="rId27" ref="G44"/>
-    <hyperlink r:id="rId28" ref="G45"/>
-    <hyperlink r:id="rId29" ref="G46"/>
-    <hyperlink r:id="rId30" ref="G47"/>
-    <hyperlink r:id="rId31" ref="G48"/>
-    <hyperlink r:id="rId32" ref="G49"/>
-    <hyperlink r:id="rId33" ref="G50"/>
-    <hyperlink r:id="rId34" ref="G51"/>
-    <hyperlink r:id="rId35" ref="G52"/>
-    <hyperlink r:id="rId36" ref="G53"/>
-    <hyperlink r:id="rId37" ref="G54"/>
-    <hyperlink r:id="rId38" ref="G55"/>
-    <hyperlink r:id="rId39" ref="G56"/>
-    <hyperlink r:id="rId40" ref="G57"/>
-    <hyperlink r:id="rId41" ref="G58"/>
-    <hyperlink r:id="rId42" ref="G59"/>
-    <hyperlink r:id="rId43" ref="G60"/>
-    <hyperlink r:id="rId44" ref="G61"/>
-    <hyperlink r:id="rId45" ref="G62"/>
-    <hyperlink r:id="rId46" ref="G63"/>
-    <hyperlink r:id="rId47" ref="G64"/>
-    <hyperlink r:id="rId48" ref="G65"/>
-    <hyperlink r:id="rId49" ref="G66"/>
-    <hyperlink r:id="rId50" ref="G67"/>
-    <hyperlink r:id="rId51" ref="G68"/>
-    <hyperlink r:id="rId52" ref="G69"/>
-    <hyperlink r:id="rId53" ref="G70"/>
-    <hyperlink r:id="rId54" ref="G71"/>
-    <hyperlink r:id="rId55" ref="G72"/>
-    <hyperlink r:id="rId56" ref="G73"/>
-    <hyperlink r:id="rId57" ref="G74"/>
-    <hyperlink r:id="rId58" ref="G75"/>
-    <hyperlink r:id="rId59" ref="G76"/>
-    <hyperlink r:id="rId60" ref="G77"/>
-    <hyperlink r:id="rId61" ref="G78"/>
-    <hyperlink r:id="rId62" ref="G79"/>
-    <hyperlink r:id="rId63" ref="G80"/>
-    <hyperlink r:id="rId64" ref="G81"/>
-    <hyperlink r:id="rId65" ref="G82"/>
-    <hyperlink r:id="rId66" ref="G83"/>
-    <hyperlink r:id="rId67" ref="G84"/>
-    <hyperlink r:id="rId68" ref="G85"/>
-    <hyperlink r:id="rId69" ref="G86"/>
-    <hyperlink r:id="rId70" ref="G87"/>
-    <hyperlink r:id="rId71" ref="G88"/>
-    <hyperlink r:id="rId72" ref="G89"/>
-    <hyperlink r:id="rId73" ref="G90"/>
-    <hyperlink r:id="rId74" ref="G91"/>
-    <hyperlink r:id="rId75" ref="G95"/>
-    <hyperlink r:id="rId76" ref="G103"/>
-    <hyperlink r:id="rId77" ref="G104"/>
-    <hyperlink r:id="rId78" ref="G105"/>
-    <hyperlink r:id="rId79" ref="G106"/>
-    <hyperlink r:id="rId80" ref="G107"/>
-    <hyperlink r:id="rId81" ref="G108"/>
-    <hyperlink r:id="rId82" ref="G109"/>
-    <hyperlink r:id="rId83" ref="G110"/>
-    <hyperlink r:id="rId84" ref="G111"/>
-    <hyperlink r:id="rId85" ref="G112"/>
-    <hyperlink r:id="rId86" ref="G113"/>
-    <hyperlink r:id="rId87" ref="G114"/>
-    <hyperlink r:id="rId88" ref="G115"/>
-    <hyperlink r:id="rId89" ref="G116"/>
+    <hyperlink r:id="rId2" location="fantasy::27" ref="G18"/>
+    <hyperlink r:id="rId3" ref="G19"/>
+    <hyperlink r:id="rId4" ref="G20"/>
+    <hyperlink r:id="rId5" ref="G21"/>
+    <hyperlink r:id="rId6" ref="G22"/>
+    <hyperlink r:id="rId7" ref="G23"/>
+    <hyperlink r:id="rId8" ref="G24"/>
+    <hyperlink r:id="rId9" ref="G25"/>
+    <hyperlink r:id="rId10" ref="G26"/>
+    <hyperlink r:id="rId11" ref="G27"/>
+    <hyperlink r:id="rId12" ref="G28"/>
+    <hyperlink r:id="rId13" ref="G29"/>
+    <hyperlink r:id="rId14" ref="G30"/>
+    <hyperlink r:id="rId15" ref="G31"/>
+    <hyperlink r:id="rId16" ref="G32"/>
+    <hyperlink r:id="rId17" ref="G33"/>
+    <hyperlink r:id="rId18" ref="G34"/>
+    <hyperlink r:id="rId19" ref="G35"/>
+    <hyperlink r:id="rId20" ref="G36"/>
+    <hyperlink r:id="rId21" ref="G37"/>
+    <hyperlink r:id="rId22" ref="G38"/>
+    <hyperlink r:id="rId23" ref="G39"/>
+    <hyperlink r:id="rId24" ref="G40"/>
+    <hyperlink r:id="rId25" ref="G41"/>
+    <hyperlink r:id="rId26" ref="G42"/>
+    <hyperlink r:id="rId27" ref="G43"/>
+    <hyperlink r:id="rId28" ref="G44"/>
+    <hyperlink r:id="rId29" ref="G45"/>
+    <hyperlink r:id="rId30" ref="G46"/>
+    <hyperlink r:id="rId31" ref="G47"/>
+    <hyperlink r:id="rId32" ref="G48"/>
+    <hyperlink r:id="rId33" ref="G49"/>
+    <hyperlink r:id="rId34" ref="G50"/>
+    <hyperlink r:id="rId35" ref="G51"/>
+    <hyperlink r:id="rId36" ref="G52"/>
+    <hyperlink r:id="rId37" ref="G53"/>
+    <hyperlink r:id="rId38" ref="G54"/>
+    <hyperlink r:id="rId39" ref="G55"/>
+    <hyperlink r:id="rId40" ref="G56"/>
+    <hyperlink r:id="rId41" ref="G57"/>
+    <hyperlink r:id="rId42" ref="G58"/>
+    <hyperlink r:id="rId43" ref="G59"/>
+    <hyperlink r:id="rId44" ref="G60"/>
+    <hyperlink r:id="rId45" ref="G61"/>
+    <hyperlink r:id="rId46" ref="G62"/>
+    <hyperlink r:id="rId47" ref="G63"/>
+    <hyperlink r:id="rId48" ref="G64"/>
+    <hyperlink r:id="rId49" ref="G65"/>
+    <hyperlink r:id="rId50" ref="G66"/>
+    <hyperlink r:id="rId51" ref="G67"/>
+    <hyperlink r:id="rId52" ref="G68"/>
+    <hyperlink r:id="rId53" ref="G69"/>
+    <hyperlink r:id="rId54" ref="G70"/>
+    <hyperlink r:id="rId55" ref="G71"/>
+    <hyperlink r:id="rId56" ref="G72"/>
+    <hyperlink r:id="rId57" ref="G73"/>
+    <hyperlink r:id="rId58" ref="G74"/>
+    <hyperlink r:id="rId59" ref="G75"/>
+    <hyperlink r:id="rId60" ref="G76"/>
+    <hyperlink r:id="rId61" ref="G77"/>
+    <hyperlink r:id="rId62" ref="G78"/>
+    <hyperlink r:id="rId63" ref="G79"/>
+    <hyperlink r:id="rId64" ref="G80"/>
+    <hyperlink r:id="rId65" ref="G81"/>
+    <hyperlink r:id="rId66" ref="G82"/>
+    <hyperlink r:id="rId67" ref="G83"/>
+    <hyperlink r:id="rId68" ref="G84"/>
+    <hyperlink r:id="rId69" ref="G85"/>
+    <hyperlink r:id="rId70" ref="G86"/>
+    <hyperlink r:id="rId71" ref="G87"/>
+    <hyperlink r:id="rId72" ref="G88"/>
+    <hyperlink r:id="rId73" ref="G89"/>
+    <hyperlink r:id="rId74" ref="G90"/>
+    <hyperlink r:id="rId75" ref="G91"/>
+    <hyperlink r:id="rId76" ref="G95"/>
+    <hyperlink r:id="rId77" ref="G100"/>
+    <hyperlink r:id="rId78" ref="G103"/>
+    <hyperlink r:id="rId79" ref="G104"/>
+    <hyperlink r:id="rId80" ref="G105"/>
+    <hyperlink r:id="rId81" ref="G106"/>
+    <hyperlink r:id="rId82" ref="G107"/>
+    <hyperlink r:id="rId83" ref="G108"/>
+    <hyperlink r:id="rId84" ref="G109"/>
+    <hyperlink r:id="rId85" ref="G110"/>
+    <hyperlink r:id="rId86" ref="G111"/>
+    <hyperlink r:id="rId87" ref="G112"/>
+    <hyperlink r:id="rId88" ref="G113"/>
+    <hyperlink r:id="rId89" ref="G114"/>
+    <hyperlink r:id="rId90" ref="G115"/>
+    <hyperlink r:id="rId91" ref="G116"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId90"/>
+  <drawing r:id="rId92"/>
+  <legacyDrawing r:id="rId93"/>
 </worksheet>
 </file>
 
@@ -6022,16 +6069,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="36.0" customHeight="1">
-      <c r="A1" s="21" t="s">
-        <v>361</v>
+      <c r="A1" s="22" t="s">
+        <v>363</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" ht="36.0" customHeight="1">
-      <c r="A2" s="22" t="s">
-        <v>362</v>
+      <c r="A2" s="23" t="s">
+        <v>364</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6043,326 +6090,326 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="23">
+      <c r="A5" s="24">
         <v>6.0</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D5" s="24"/>
+      <c r="B5" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" ht="25.5" customHeight="1">
-      <c r="A6" s="23">
+      <c r="A6" s="24">
         <v>6.0</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" ht="25.5" customHeight="1">
+      <c r="A7" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" ht="25.5" customHeight="1">
+      <c r="A8" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" ht="25.5" customHeight="1">
+      <c r="A9" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" ht="25.5" customHeight="1">
+      <c r="A10" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" ht="25.5" customHeight="1">
+      <c r="A11" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" ht="25.5" customHeight="1">
+      <c r="A12" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1">
+      <c r="A13" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="A14" s="24">
+        <v>6.0</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" ht="25.5" customHeight="1">
+      <c r="A15" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B15" s="28" t="s">
         <v>368</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D6" s="24"/>
-    </row>
-    <row r="7" ht="25.5" customHeight="1">
-      <c r="A7" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="24" t="s">
+      <c r="C15" s="29" t="s">
         <v>369</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D7" s="24"/>
-    </row>
-    <row r="8" ht="25.5" customHeight="1">
-      <c r="A8" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" ht="25.5" customHeight="1">
+      <c r="A16" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" ht="25.5" customHeight="1">
-      <c r="A9" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B9" s="24" t="s">
+      <c r="C16" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" ht="25.5" customHeight="1">
+      <c r="A17" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" ht="25.5" customHeight="1">
-      <c r="A10" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B10" s="24" t="s">
+      <c r="C17" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" ht="25.5" customHeight="1">
+      <c r="A18" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D10" s="24"/>
-    </row>
-    <row r="11" ht="25.5" customHeight="1">
-      <c r="A11" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B11" s="24" t="s">
+      <c r="C18" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" ht="25.5" customHeight="1">
+      <c r="A19" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D11" s="24"/>
-    </row>
-    <row r="12" ht="25.5" customHeight="1">
-      <c r="A12" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B12" s="24" t="s">
+      <c r="C19" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" ht="25.5" customHeight="1">
+      <c r="A20" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B13" s="24" t="s">
+      <c r="C20" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" ht="25.5" customHeight="1">
+      <c r="A21" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B21" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="B14" s="24" t="s">
+      <c r="C21" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" ht="25.5" customHeight="1">
+      <c r="A22" s="27">
+        <v>7.0</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>376</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" ht="25.5" customHeight="1">
-      <c r="A15" s="26">
+      <c r="C22" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" ht="25.5" customHeight="1">
+      <c r="A23" s="27">
         <v>7.0</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" ht="25.5" customHeight="1">
-      <c r="A16" s="26">
+      <c r="B23" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" ht="25.5" customHeight="1">
+      <c r="A24" s="27">
         <v>7.0</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>368</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" ht="25.5" customHeight="1">
-      <c r="A17" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B17" s="27" t="s">
+      <c r="B24" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>369</v>
       </c>
-      <c r="C17" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D17" s="27"/>
-    </row>
-    <row r="18" ht="25.5" customHeight="1">
-      <c r="A18" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>370</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" ht="25.5" customHeight="1">
-      <c r="A19" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>371</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D19" s="27"/>
-    </row>
-    <row r="20" ht="25.5" customHeight="1">
-      <c r="A20" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>372</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D20" s="27"/>
-    </row>
-    <row r="21" ht="25.5" customHeight="1">
-      <c r="A21" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>373</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" ht="25.5" customHeight="1">
-      <c r="A22" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>374</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D22" s="27"/>
-    </row>
-    <row r="23" ht="25.5" customHeight="1">
-      <c r="A23" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>375</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D23" s="27"/>
-    </row>
-    <row r="24" ht="25.5" customHeight="1">
-      <c r="A24" s="26">
-        <v>7.0</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>376</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" ht="25.5" customHeight="1">
-      <c r="A25" s="29">
+      <c r="A25" s="30">
         <v>8.0</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>377</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>378</v>
-      </c>
-      <c r="D25" s="30"/>
+      <c r="B25" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>380</v>
+      </c>
+      <c r="D25" s="31"/>
     </row>
     <row r="26" ht="25.5" customHeight="1">
-      <c r="A26" s="29">
+      <c r="A26" s="30">
         <v>8.0</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>379</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>380</v>
-      </c>
-      <c r="D26" s="30"/>
+      <c r="B26" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="D26" s="31"/>
     </row>
     <row r="27" ht="25.5" customHeight="1">
-      <c r="A27" s="29">
+      <c r="A27" s="30">
         <v>8.0</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>381</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>382</v>
-      </c>
-      <c r="D27" s="30"/>
+      <c r="B27" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" ht="25.5" customHeight="1">
-      <c r="A28" s="29">
+      <c r="A28" s="30">
         <v>8.0</v>
       </c>
-      <c r="B28" s="30" t="s">
-        <v>383</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>384</v>
-      </c>
-      <c r="D28" s="30"/>
+      <c r="B28" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>386</v>
+      </c>
+      <c r="D28" s="31"/>
     </row>
     <row r="29" ht="25.5" customHeight="1">
-      <c r="A29" s="29">
+      <c r="A29" s="30">
         <v>8.0</v>
       </c>
-      <c r="B29" s="30" t="s">
-        <v>385</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>386</v>
-      </c>
-      <c r="D29" s="30"/>
+      <c r="B29" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="D29" s="31"/>
     </row>
     <row r="30" ht="25.5" customHeight="1">
-      <c r="A30" s="29">
+      <c r="A30" s="30">
         <v>8.0</v>
       </c>
-      <c r="B30" s="30" t="s">
-        <v>387</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>388</v>
-      </c>
-      <c r="D30" s="30"/>
+      <c r="B30" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="D30" s="31"/>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>
@@ -7362,234 +7409,234 @@
   </cols>
   <sheetData>
     <row r="1" ht="39.75" customHeight="1">
-      <c r="A1" s="32" t="s">
-        <v>389</v>
+      <c r="A1" s="33" t="s">
+        <v>391</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" ht="25.5" customHeight="1">
-      <c r="A2" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="B2" s="34"/>
+      <c r="A2" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" ht="29.25" customHeight="1">
-      <c r="A3" s="35" t="s">
-        <v>391</v>
+      <c r="A3" s="36" t="s">
+        <v>393</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" ht="25.5" customHeight="1"/>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="33" t="s">
-        <v>393</v>
-      </c>
-      <c r="B5" s="34"/>
+      <c r="A5" s="34" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="35"/>
     </row>
     <row r="6" ht="18.0" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" ht="18.0" customHeight="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" ht="18.0" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" ht="18.0" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" ht="79.5" customHeight="1">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" ht="18.0" customHeight="1">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" ht="18.0" customHeight="1">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" ht="25.5" customHeight="1"/>
     <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="33" t="s">
-        <v>401</v>
-      </c>
-      <c r="B14" s="34"/>
+      <c r="A14" s="34" t="s">
+        <v>403</v>
+      </c>
+      <c r="B14" s="35"/>
     </row>
     <row r="15" ht="18.0" customHeight="1">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" ht="18.0" customHeight="1">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" ht="18.0" customHeight="1">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" ht="18.0" customHeight="1">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="19" ht="25.5" customHeight="1"/>
     <row r="20" ht="25.5" customHeight="1">
-      <c r="A20" s="33" t="s">
-        <v>406</v>
-      </c>
-      <c r="B20" s="34"/>
+      <c r="A20" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="B20" s="35"/>
     </row>
     <row r="21" ht="18.0" customHeight="1">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" ht="18.0" customHeight="1">
-      <c r="A22" s="35" t="s">
-        <v>408</v>
+      <c r="A22" s="36" t="s">
+        <v>410</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" ht="18.0" customHeight="1">
-      <c r="A23" s="35" t="s">
-        <v>364</v>
+      <c r="A23" s="36" t="s">
+        <v>366</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" ht="18.0" customHeight="1">
-      <c r="A24" s="35" t="s">
-        <v>411</v>
+      <c r="A24" s="36" t="s">
+        <v>413</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" ht="25.5" customHeight="1"/>
     <row r="26" ht="25.5" customHeight="1">
-      <c r="A26" s="33" t="s">
-        <v>413</v>
-      </c>
-      <c r="B26" s="34"/>
+      <c r="A26" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="B26" s="35"/>
     </row>
     <row r="27" ht="18.0" customHeight="1">
-      <c r="A27" s="35" t="s">
-        <v>414</v>
+      <c r="A27" s="36" t="s">
+        <v>416</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" ht="18.0" customHeight="1">
-      <c r="A28" s="35" t="s">
-        <v>416</v>
+      <c r="A28" s="36" t="s">
+        <v>418</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" ht="18.0" customHeight="1">
-      <c r="A29" s="35" t="s">
-        <v>418</v>
+      <c r="A29" s="36" t="s">
+        <v>420</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" ht="18.0" customHeight="1">
-      <c r="A30" s="35" t="s">
-        <v>420</v>
+      <c r="A30" s="36" t="s">
+        <v>422</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" ht="25.5" customHeight="1"/>
     <row r="32" ht="25.5" customHeight="1">
-      <c r="A32" s="33" t="s">
-        <v>422</v>
-      </c>
-      <c r="B32" s="34"/>
+      <c r="A32" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="B32" s="35"/>
     </row>
     <row r="33" ht="18.0" customHeight="1">
-      <c r="A33" s="35" t="s">
-        <v>423</v>
+      <c r="A33" s="36" t="s">
+        <v>425</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34" ht="18.0" customHeight="1">
-      <c r="A34" s="35" t="s">
-        <v>425</v>
+      <c r="A34" s="36" t="s">
+        <v>427</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" ht="18.0" customHeight="1">
-      <c r="A35" s="35" t="s">
-        <v>427</v>
+      <c r="A35" s="36" t="s">
+        <v>429</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>

</xml_diff>